<commit_message>
fix: move i18n to csv script
</commit_message>
<xml_diff>
--- a/packages/react-i18n-ast/public/locales/zh/translation.xlsx
+++ b/packages/react-i18n-ast/public/locales/zh/translation.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,71 +412,47 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>咕咕鸡</v>
+        <v>武汉</v>
       </c>
       <c r="B2" t="str">
-        <v>咕咕鸡</v>
+        <v>武汉[chinese]</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>跑步</v>
+        <v>name_1718273788838</v>
       </c>
       <c r="B3" t="str">
-        <v>跑步</v>
+        <v>{{name}}</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>是个boy</v>
+        <v>address_1718273788839</v>
       </c>
       <c r="B4" t="str">
-        <v>是个boy</v>
+        <v>{{address}}</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>关于</v>
+        <v>我的名字：</v>
       </c>
       <c r="B5" t="str">
-        <v>关于</v>
+        <v>我的名字：[chinese]</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>我的名字：</v>
+        <v>东湖</v>
       </c>
       <c r="B6" t="str">
-        <v>我的名字：</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>网球</v>
-      </c>
-      <c r="B7" t="str">
-        <v>网球</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>我的兴趣</v>
-      </c>
-      <c r="B8" t="str">
-        <v>我的兴趣</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>请输入你的年龄</v>
-      </c>
-      <c r="B9" t="str">
-        <v>请输入你的年龄</v>
+        <v>东湖[chinese]</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>